<commit_message>
Modify program according new requirement.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
   <si>
     <t>Date</t>
   </si>
@@ -36,6 +36,11 @@
   <si>
     <t>Try use mutile-thread to get the tranasction data, but failed becase of WIND API don't support.</t>
   </si>
+  <si>
+    <t>1.Resolve the new account can't be logged in, but still failed.
+2.Modify the algorithm according new requirement.
+3.Run the program to calculate the running time.</t>
+  </si>
 </sst>
 </file>
 
@@ -47,7 +52,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -56,6 +61,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -63,16 +69,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -84,9 +121,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -95,65 +168,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,9 +181,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -184,6 +213,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -191,24 +228,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,6 +244,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -241,114 +406,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -361,36 +418,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -398,12 +425,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,17 +438,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -448,16 +469,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,30 +518,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -514,161 +526,176 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="49" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="49" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyFont="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1048,73 +1075,94 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="10.375"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="107.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>42511</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>42513</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>42514</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>42515</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="6" ht="42.75" spans="1:3">
+      <c r="A6" s="3">
+        <v>42516</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3"/>
+      <c r="B7"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3"/>
+      <c r="B8"/>
+      <c r="C8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
For the first task.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8355" tabRatio="500"/>
+    <workbookView windowWidth="25095" windowHeight="12570" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,28 @@
     <t>1.Resolve the new account can't be logged in, but still failed.
 2.Modify the algorithm according new requirement.
 3.Run the program to calculate the running time.</t>
+  </si>
+  <si>
+    <t>1.Test the new accout. 
+2.Generate the exe program.</t>
+  </si>
+  <si>
+    <t>test the account</t>
+  </si>
+  <si>
+    <t>release an exe using new accunt</t>
+  </si>
+  <si>
+    <t>fix the bug without TDBAPI.dll</t>
+  </si>
+  <si>
+    <t>reply mail, discuss solution</t>
+  </si>
+  <si>
+    <t>total: 28 hours</t>
+  </si>
+  <si>
+    <t>implement the new requirement.</t>
   </si>
 </sst>
 </file>
@@ -52,7 +74,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,7 +91,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -77,99 +98,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,45 +129,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -229,7 +137,113 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,103 +258,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,79 +432,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,6 +449,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -464,6 +487,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,24 +541,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -526,15 +549,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -543,10 +557,10 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -555,133 +569,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -689,13 +703,13 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="49"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="49" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="49" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -749,6 +763,7 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
     <cellStyle name="Normal" xfId="49"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -1075,27 +1090,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="10.375"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="107.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1115,7 +1130,7 @@
         <v>42513</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -1154,15 +1169,87 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3"/>
-      <c r="B7"/>
-      <c r="C7" s="6"/>
+    <row r="7" ht="28.5" spans="1:3">
+      <c r="A7" s="3">
+        <v>42527</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3"/>
-      <c r="B8"/>
-      <c r="C8" s="6"/>
+      <c r="A8" s="3">
+        <v>42541</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>42544</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>42545</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>42180</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>42548</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" spans="1:3">
+      <c r="A14" s="6">
+        <v>42549</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
finish get data of 2016/4.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>implement the new requirement.</t>
+  </si>
+  <si>
+    <t>fix a bug.</t>
+  </si>
+  <si>
+    <t>check with wind about the lose connection issue.</t>
   </si>
 </sst>
 </file>
@@ -74,7 +80,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,7 +97,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -99,16 +121,122 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -119,135 +247,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -258,37 +257,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,139 +425,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,6 +448,65 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -477,39 +535,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -523,32 +548,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -557,10 +556,10 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -569,147 +568,145 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="49"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="49" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="49" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1090,10 +1087,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1115,73 +1112,73 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>42511</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>42513</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>42514</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>42515</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" ht="42.75" spans="1:3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>42516</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" ht="28.5" spans="1:3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>42527</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>42541</v>
       </c>
       <c r="B8">
@@ -1192,7 +1189,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>42544</v>
       </c>
       <c r="B9">
@@ -1203,7 +1200,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>42545</v>
       </c>
       <c r="B10">
@@ -1214,7 +1211,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>42180</v>
       </c>
       <c r="B11">
@@ -1230,7 +1227,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>42548</v>
       </c>
       <c r="B13">
@@ -1240,15 +1237,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" s="2" customFormat="1" spans="1:3">
-      <c r="A14" s="6">
+    <row r="14" customFormat="1" spans="1:3">
+      <c r="A14" s="2">
         <v>42549</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2">
+        <v>42550</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2">
+        <v>42551</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>